<commit_message>
Updating all necessary files of CAD. Also fixed an issue in the body assembly with the custom acrylic backplate, updated the parts list and build doc to reflect this change. Added breif section in corner steering for 3D printed encoder mount ordering
</commit_message>
<xml_diff>
--- a/Mechanical/Body Assembly/Body Assembly Parts List.xlsx
+++ b/Mechanical/Body Assembly/Body Assembly Parts List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejunkins\Desktop\open_source_rover\Documentation\Mechanical Assembly\Body Assembly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejunkins\Desktop\osr\Mechanical\Body Assembly\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Body" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Body!$A$1:$K$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Body!$A$1:$K$13</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="101">
   <si>
     <t>Part</t>
   </si>
@@ -173,18 +173,9 @@
     <t>S24</t>
   </si>
   <si>
-    <t>3003 Aluminum Sheet</t>
-  </si>
-  <si>
-    <t>MetalsDepot</t>
-  </si>
-  <si>
     <t>S28</t>
   </si>
   <si>
-    <t>.090 (3/32) thick - Custom 8x11 cut</t>
-  </si>
-  <si>
     <t>9 x 12 Inch Aluminum Plate</t>
   </si>
   <si>
@@ -321,6 +312,24 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Sculpteo</t>
+  </si>
+  <si>
+    <t>S37B</t>
+  </si>
+  <si>
+    <t>https://www.sculpteo.com/</t>
+  </si>
+  <si>
+    <t>Custom Acrylic Back plate*</t>
+  </si>
+  <si>
+    <t>Custom Acrylic Electronics Board*</t>
+  </si>
+  <si>
+    <t>*Files for Custom Acrylic are found under the Laser Cut parts folder</t>
   </si>
 </sst>
 </file>
@@ -386,7 +395,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -397,6 +406,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -495,7 +510,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -541,9 +556,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -599,6 +611,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -881,29 +900,29 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:Z26"/>
+  <dimension ref="A1:Z28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="40.73046875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10.59765625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10.3984375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.86328125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.59765625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.73046875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.3984375" style="4" customWidth="1"/>
     <col min="9" max="9" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="39.85546875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="20.265625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="39.86328125" style="4" customWidth="1"/>
     <col min="12" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="36.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -938,7 +957,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
         <v>11</v>
       </c>
@@ -967,14 +986,14 @@
         <v>4.49</v>
       </c>
       <c r="J2" s="11">
-        <f t="shared" ref="J2:J24" si="0">B2/D2*I2</f>
+        <f t="shared" ref="J2:J25" si="0">B2/D2*I2</f>
         <v>4.49</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
@@ -1010,7 +1029,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>21</v>
       </c>
@@ -1046,7 +1065,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
         <v>25</v>
       </c>
@@ -1065,7 +1084,7 @@
       <c r="F5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="17" t="s">
         <v>27</v>
       </c>
       <c r="H5" s="8" t="s">
@@ -1082,7 +1101,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="10" t="s">
         <v>29</v>
       </c>
@@ -1118,7 +1137,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="10" t="s">
         <v>33</v>
       </c>
@@ -1154,7 +1173,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
         <v>36</v>
       </c>
@@ -1190,7 +1209,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="13" t="s">
         <v>39</v>
       </c>
@@ -1226,7 +1245,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="10" t="s">
         <v>42</v>
       </c>
@@ -1262,7 +1281,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="8" t="s">
         <v>46</v>
       </c>
@@ -1298,51 +1317,51 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B12" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="8">
-        <v>1</v>
-      </c>
-      <c r="D12" s="17">
+        <v>2</v>
+      </c>
+      <c r="D12" s="9">
         <v>1</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G12" s="10" t="s">
-        <v>51</v>
+      <c r="G12" s="10">
+        <v>585006</v>
       </c>
       <c r="H12" s="14" t="s">
         <v>32</v>
       </c>
       <c r="I12" s="11">
-        <v>9.6999999999999993</v>
+        <v>16.989999999999998</v>
       </c>
       <c r="J12" s="11">
         <f t="shared" si="0"/>
-        <v>9.6999999999999993</v>
+        <v>33.979999999999997</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="8" t="s">
         <v>52</v>
       </c>
       <c r="B13" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" s="9">
         <v>1</v>
@@ -1354,214 +1373,215 @@
         <v>53</v>
       </c>
       <c r="G13" s="10">
-        <v>585006</v>
+        <v>585004</v>
       </c>
       <c r="H13" s="14" t="s">
         <v>32</v>
       </c>
       <c r="I13" s="11">
-        <v>16.989999999999998</v>
+        <v>13.99</v>
       </c>
       <c r="J13" s="11">
         <f t="shared" si="0"/>
-        <v>33.979999999999997</v>
+        <v>41.97</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="13">
+        <v>12</v>
+      </c>
+      <c r="C14" s="13">
+        <v>12</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="11">
+        <v>0.23</v>
+      </c>
+      <c r="J14" s="11">
+        <f t="shared" si="0"/>
+        <v>2.7600000000000002</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="8">
         <v>4</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C15" s="8">
         <v>4</v>
       </c>
-      <c r="D14" s="9">
-        <v>1</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G14" s="10">
-        <v>585004</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="I14" s="11">
-        <v>13.99</v>
-      </c>
-      <c r="J14" s="11">
-        <f t="shared" si="0"/>
-        <v>55.96</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="13">
-        <v>12</v>
-      </c>
-      <c r="C15" s="13">
-        <v>12</v>
-      </c>
       <c r="D15" s="9">
         <v>1</v>
       </c>
-      <c r="E15" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>59</v>
+      <c r="E15" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>15</v>
       </c>
       <c r="I15" s="11">
-        <v>0.23</v>
+        <v>0.3</v>
       </c>
       <c r="J15" s="11">
         <f t="shared" si="0"/>
-        <v>2.7600000000000002</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1.2</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L15" s="7"/>
+    </row>
+    <row r="16" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B16" s="8">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="C16" s="8">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D16" s="9">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16" s="19" t="s">
         <v>64</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>65</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>15</v>
       </c>
       <c r="I16" s="11">
-        <v>0.3</v>
+        <v>1.17</v>
       </c>
       <c r="J16" s="11">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1.17</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L16" s="7"/>
     </row>
-    <row r="17" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>66</v>
+    <row r="17" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="B17" s="8">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="C17" s="8">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D17" s="9">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G17" s="18" t="s">
         <v>68</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>15</v>
       </c>
       <c r="I17" s="11">
-        <v>1.17</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="J17" s="11">
         <f t="shared" si="0"/>
-        <v>1.17</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L17" s="7"/>
     </row>
-    <row r="18" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="8">
-        <v>5</v>
-      </c>
-      <c r="C18" s="8">
-        <v>3</v>
+        <v>71</v>
+      </c>
+      <c r="B18" s="13">
+        <v>12</v>
+      </c>
+      <c r="C18" s="13">
+        <v>8</v>
       </c>
       <c r="D18" s="9">
-        <v>5</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G18" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="13" t="s">
         <v>72</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>73</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>15</v>
       </c>
       <c r="I18" s="11">
-        <v>2.4700000000000002</v>
+        <v>0.23</v>
       </c>
       <c r="J18" s="11">
         <f t="shared" si="0"/>
-        <v>2.4700000000000002</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>73</v>
+        <v>2.7600000000000002</v>
+      </c>
+      <c r="K18" s="34" t="s">
+        <v>74</v>
       </c>
       <c r="L18" s="7"/>
     </row>
-    <row r="19" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B19" s="13">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C19" s="13">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D19" s="9">
         <v>1</v>
@@ -1570,229 +1590,265 @@
         <v>12</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="G19" s="18" t="s">
         <v>76</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>77</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>15</v>
       </c>
       <c r="I19" s="11">
-        <v>0.23</v>
+        <v>0.27</v>
       </c>
       <c r="J19" s="11">
         <f t="shared" si="0"/>
-        <v>2.7600000000000002</v>
-      </c>
-      <c r="K19" s="35" t="s">
-        <v>77</v>
+        <v>4.32</v>
+      </c>
+      <c r="K19" s="34" t="s">
+        <v>78</v>
       </c>
       <c r="L19" s="7"/>
-    </row>
-    <row r="20" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+    </row>
+    <row r="20" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B20" s="13">
-        <v>16</v>
-      </c>
-      <c r="C20" s="13">
-        <v>12</v>
+        <v>79</v>
+      </c>
+      <c r="B20" s="8">
+        <v>12</v>
+      </c>
+      <c r="C20" s="8">
+        <v>8</v>
       </c>
       <c r="D20" s="9">
         <v>1</v>
       </c>
-      <c r="E20" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="G20" s="18" t="s">
+      <c r="E20" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>80</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>81</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>15</v>
       </c>
       <c r="I20" s="11">
-        <v>0.27</v>
+        <v>0.37</v>
       </c>
       <c r="J20" s="11">
         <f t="shared" si="0"/>
-        <v>4.32</v>
-      </c>
-      <c r="K20" s="35" t="s">
-        <v>81</v>
+        <v>4.4399999999999995</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>82</v>
       </c>
       <c r="L20" s="7"/>
       <c r="X20" s="7"/>
       <c r="Y20" s="7"/>
       <c r="Z20" s="7"/>
     </row>
-    <row r="21" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="B21" s="8">
-        <v>12</v>
-      </c>
-      <c r="C21" s="8">
-        <v>8</v>
-      </c>
-      <c r="D21" s="9">
-        <v>1</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="8" t="s">
+    <row r="21" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="G21" s="18" t="s">
+      <c r="B21" s="20">
+        <v>6</v>
+      </c>
+      <c r="C21" s="20">
+        <v>4</v>
+      </c>
+      <c r="D21" s="21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="H21" s="8" t="s">
+      <c r="G21" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="H21" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="I21" s="11">
-        <v>0.37</v>
-      </c>
-      <c r="J21" s="11">
-        <f t="shared" si="0"/>
-        <v>4.4399999999999995</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>85</v>
+      <c r="I21" s="24">
+        <v>0.48</v>
+      </c>
+      <c r="J21" s="24">
+        <f t="shared" si="0"/>
+        <v>2.88</v>
+      </c>
+      <c r="K21" s="25" t="s">
+        <v>86</v>
       </c>
       <c r="L21" s="7"/>
       <c r="X21" s="7"/>
       <c r="Y21" s="7"/>
       <c r="Z21" s="7"/>
     </row>
-    <row r="22" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B22" s="21">
-        <v>6</v>
-      </c>
-      <c r="C22" s="21">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A22" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="27">
+        <v>100</v>
+      </c>
+      <c r="C22" s="27">
         <v>4</v>
       </c>
-      <c r="D22" s="22">
-        <v>1</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="21" t="s">
+      <c r="D22" s="27">
+        <v>100</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="30">
+        <v>6.33</v>
+      </c>
+      <c r="J22" s="30">
+        <f t="shared" si="0"/>
+        <v>6.33</v>
+      </c>
+      <c r="K22" s="31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A23" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="G22" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="H22" s="24" t="s">
+      <c r="B23" s="27">
+        <v>4</v>
+      </c>
+      <c r="C23" s="27">
+        <v>2</v>
+      </c>
+      <c r="D23" s="27">
+        <v>1</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="H23" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="I22" s="25">
-        <v>0.48</v>
-      </c>
-      <c r="J22" s="25">
-        <f t="shared" si="0"/>
-        <v>2.88</v>
-      </c>
-      <c r="K22" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="L22" s="7"/>
-      <c r="X22" s="7"/>
-      <c r="Y22" s="7"/>
-      <c r="Z22" s="7"/>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" s="28">
+      <c r="I23" s="30">
+        <v>0.96</v>
+      </c>
+      <c r="J23" s="30">
+        <f t="shared" si="0"/>
+        <v>3.84</v>
+      </c>
+      <c r="K23" s="31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A24" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="27">
+        <v>1</v>
+      </c>
+      <c r="C24" s="27">
+        <v>1</v>
+      </c>
+      <c r="D24" s="27">
+        <v>1</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G24" s="36"/>
+      <c r="H24" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="I24" s="30">
+        <v>11.75</v>
+      </c>
+      <c r="J24" s="30">
+        <f t="shared" si="0"/>
+        <v>11.75</v>
+      </c>
+      <c r="K24" s="31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A25" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" s="27">
+        <v>1</v>
+      </c>
+      <c r="C25" s="27">
+        <v>1</v>
+      </c>
+      <c r="D25" s="27">
+        <v>1</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="G25" s="36"/>
+      <c r="H25" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="30">
+        <v>15.25</v>
+      </c>
+      <c r="J25" s="30">
+        <f t="shared" si="0"/>
+        <v>15.25</v>
+      </c>
+      <c r="K25" s="31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A27" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="28">
-        <v>4</v>
-      </c>
-      <c r="D23" s="28">
-        <v>100</v>
-      </c>
-      <c r="E23" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="G23" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="H23" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" s="31">
-        <v>6.33</v>
-      </c>
-      <c r="J23" s="31">
-        <f t="shared" si="0"/>
-        <v>6.33</v>
-      </c>
-      <c r="K23" s="32" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A24" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="B24" s="28">
-        <v>4</v>
-      </c>
-      <c r="C24" s="28">
-        <v>2</v>
-      </c>
-      <c r="D24" s="28">
-        <v>1</v>
-      </c>
-      <c r="E24" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="28" t="s">
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="J28" s="35">
+        <f>SUM(J2:J25)</f>
+        <v>240.37999999999994</v>
+      </c>
+      <c r="K28" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G24" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="H24" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" s="31">
-        <v>0.96</v>
-      </c>
-      <c r="J24" s="31">
-        <f t="shared" si="0"/>
-        <v>3.84</v>
-      </c>
-      <c r="K24" s="32" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="J26" s="36">
-        <f>SUM(J2:J24)</f>
-        <v>237.06999999999996</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>97</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K14">
+  <autoFilter ref="A1:K13">
     <filterColumn colId="7">
       <filters>
         <filter val="Structural"/>
@@ -1803,22 +1859,23 @@
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="K13" r:id="rId1"/>
-    <hyperlink ref="K14" r:id="rId2"/>
+    <hyperlink ref="K12" r:id="rId1"/>
+    <hyperlink ref="K13" r:id="rId2"/>
     <hyperlink ref="K11" r:id="rId3"/>
-    <hyperlink ref="K12" r:id="rId4"/>
-    <hyperlink ref="K3" r:id="rId5" location="90631A007"/>
-    <hyperlink ref="K5" r:id="rId6" location="96006A252"/>
-    <hyperlink ref="K6" r:id="rId7"/>
-    <hyperlink ref="K10" r:id="rId8" location="368=229"/>
-    <hyperlink ref="K7" r:id="rId9"/>
-    <hyperlink ref="K22" r:id="rId10" location="95947A007"/>
-    <hyperlink ref="K23" r:id="rId11" location="91251A076"/>
-    <hyperlink ref="K24" r:id="rId12" location="93330A252"/>
-    <hyperlink ref="K19" r:id="rId13" location="91780A162"/>
-    <hyperlink ref="K20" r:id="rId14" location="91780A164"/>
+    <hyperlink ref="K3" r:id="rId4" location="90631A007"/>
+    <hyperlink ref="K5" r:id="rId5" location="96006A252"/>
+    <hyperlink ref="K6" r:id="rId6"/>
+    <hyperlink ref="K10" r:id="rId7" location="368=229"/>
+    <hyperlink ref="K7" r:id="rId8"/>
+    <hyperlink ref="K21" r:id="rId9" location="95947A007"/>
+    <hyperlink ref="K22" r:id="rId10" location="91251A076"/>
+    <hyperlink ref="K23" r:id="rId11" location="93330A252"/>
+    <hyperlink ref="K18" r:id="rId12" location="91780A162"/>
+    <hyperlink ref="K19" r:id="rId13" location="91780A164"/>
+    <hyperlink ref="K24" r:id="rId14"/>
+    <hyperlink ref="K25" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding disclaimer and copyright to the parts lists docs
</commit_message>
<xml_diff>
--- a/Mechanical/Body Assembly/Body Assembly Parts List.xlsx
+++ b/Mechanical/Body Assembly/Body Assembly Parts List.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Body" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Body!$A$1:$K$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Body!$A$4:$K$16</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="104">
   <si>
     <t>Part</t>
   </si>
@@ -330,6 +330,15 @@
   </si>
   <si>
     <t>*Files for Custom Acrylic are found under the Laser Cut parts folder</t>
+  </si>
+  <si>
+    <t>The cost information contained in this document is of a budgetary and planning nature and is intended for informational purposes only.  It does not constitute a commitment on the part of JPL and/or Caltech.</t>
+  </si>
+  <si>
+    <t>Author: Eric Junkins, Jet Propulsion Laboratory, California Institute of Technology</t>
+  </si>
+  <si>
+    <t>© 2018 California Institute of Technology. Government sponsorship acknowledged</t>
   </si>
 </sst>
 </file>
@@ -415,7 +424,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -505,12 +514,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -617,6 +644,30 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -900,10 +951,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:Z28"/>
+  <dimension ref="A1:Z31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A3" sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -922,933 +973,981 @@
     <col min="12" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="36.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+    </row>
+    <row r="2" spans="1:12" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+    </row>
+    <row r="3" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+    </row>
+    <row r="4" spans="1:12" ht="36.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="8">
-        <v>100</v>
-      </c>
-      <c r="C2" s="8">
-        <v>34</v>
-      </c>
-      <c r="D2" s="9">
-        <v>100</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="11">
-        <v>4.49</v>
-      </c>
-      <c r="J2" s="11">
-        <f t="shared" ref="J2:J25" si="0">B2/D2*I2</f>
-        <v>4.49</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="8">
-        <v>100</v>
-      </c>
-      <c r="C3" s="8">
-        <v>32</v>
-      </c>
-      <c r="D3" s="9">
-        <v>100</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="11">
-        <v>2.61</v>
-      </c>
-      <c r="J3" s="11">
-        <f t="shared" si="0"/>
-        <v>2.61</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="8">
-        <v>100</v>
-      </c>
-      <c r="C4" s="8">
-        <v>16</v>
-      </c>
-      <c r="D4" s="9">
-        <v>100</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="11">
-        <v>4.71</v>
-      </c>
-      <c r="J4" s="11">
-        <f t="shared" si="0"/>
-        <v>4.71</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="13">
-        <v>50</v>
-      </c>
-      <c r="C5" s="13">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="B5" s="8">
+        <v>100</v>
+      </c>
+      <c r="C5" s="8">
+        <v>34</v>
       </c>
       <c r="D5" s="9">
-        <v>50</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>27</v>
+        <v>100</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>15</v>
       </c>
       <c r="I5" s="11">
-        <v>5.85</v>
+        <v>4.49</v>
       </c>
       <c r="J5" s="11">
-        <f t="shared" si="0"/>
-        <v>5.85</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>28</v>
+        <f t="shared" ref="J5:J28" si="0">B5/D5*I5</f>
+        <v>4.49</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A6" s="10" t="s">
-        <v>29</v>
+      <c r="A6" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="B6" s="8">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="C6" s="8">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="D6" s="9">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="10">
-        <v>585440</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>32</v>
+        <v>18</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="I6" s="11">
-        <v>2.99</v>
+        <v>2.61</v>
       </c>
       <c r="J6" s="11">
         <f t="shared" si="0"/>
-        <v>11.96</v>
+        <v>2.61</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A7" s="10" t="s">
-        <v>33</v>
+      <c r="A7" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="B7" s="8">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="C7" s="8">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D7" s="9">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="10">
-        <v>535118</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>32</v>
+        <v>22</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="I7" s="11">
-        <v>6.99</v>
+        <v>4.71</v>
       </c>
       <c r="J7" s="11">
         <f t="shared" si="0"/>
-        <v>13.98</v>
+        <v>4.71</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B8" s="13">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="C8" s="13">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D8" s="9">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="E8" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="11">
+        <v>5.85</v>
+      </c>
+      <c r="J8" s="11">
+        <f t="shared" si="0"/>
+        <v>5.85</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="8">
+        <v>4</v>
+      </c>
+      <c r="C9" s="8">
+        <v>4</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="15">
-        <v>585470</v>
-      </c>
-      <c r="H8" s="13" t="s">
+      <c r="F9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="10">
+        <v>585440</v>
+      </c>
+      <c r="H9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="I8" s="11">
-        <v>5.99</v>
-      </c>
-      <c r="J8" s="11">
-        <f t="shared" si="0"/>
-        <v>47.92</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="13">
-        <v>1</v>
-      </c>
-      <c r="C9" s="13">
-        <v>1</v>
-      </c>
-      <c r="D9" s="9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="16">
-        <v>635252</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>32</v>
-      </c>
       <c r="I9" s="11">
-        <v>1.49</v>
+        <v>2.99</v>
       </c>
       <c r="J9" s="11">
         <f t="shared" si="0"/>
-        <v>1.49</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>41</v>
+        <v>11.96</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="10" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B10" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="9">
         <v>1</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>44</v>
+        <v>34</v>
+      </c>
+      <c r="G10" s="10">
+        <v>535118</v>
       </c>
       <c r="H10" s="14" t="s">
         <v>32</v>
       </c>
       <c r="I10" s="11">
-        <v>2.2599999999999998</v>
+        <v>6.99</v>
       </c>
       <c r="J10" s="11">
         <f t="shared" si="0"/>
-        <v>2.2599999999999998</v>
+        <v>13.98</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="8">
-        <v>1</v>
-      </c>
-      <c r="C11" s="8">
-        <v>1</v>
+        <v>36</v>
+      </c>
+      <c r="B11" s="13">
+        <v>16</v>
+      </c>
+      <c r="C11" s="13">
+        <v>16</v>
       </c>
       <c r="D11" s="9">
-        <v>1</v>
-      </c>
-      <c r="E11" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="10">
-        <v>545512</v>
-      </c>
-      <c r="H11" s="14" t="s">
+      <c r="F11" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="15">
+        <v>585470</v>
+      </c>
+      <c r="H11" s="13" t="s">
         <v>32</v>
       </c>
       <c r="I11" s="11">
-        <v>9.99</v>
+        <v>5.99</v>
       </c>
       <c r="J11" s="11">
         <f t="shared" si="0"/>
-        <v>9.99</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A12" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="8">
-        <v>2</v>
-      </c>
-      <c r="C12" s="8">
-        <v>2</v>
+        <v>47.92</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="13">
+        <v>1</v>
+      </c>
+      <c r="C12" s="13">
+        <v>1</v>
       </c>
       <c r="D12" s="9">
         <v>1</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12" s="10">
-        <v>585006</v>
-      </c>
-      <c r="H12" s="14" t="s">
+      <c r="F12" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="16">
+        <v>635252</v>
+      </c>
+      <c r="H12" s="13" t="s">
         <v>32</v>
       </c>
       <c r="I12" s="11">
-        <v>16.989999999999998</v>
+        <v>1.49</v>
       </c>
       <c r="J12" s="11">
         <f t="shared" si="0"/>
-        <v>33.979999999999997</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>51</v>
+        <v>1.49</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A13" s="8" t="s">
-        <v>52</v>
+      <c r="A13" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="B13" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13" s="9">
         <v>1</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="10">
-        <v>585004</v>
+        <v>43</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="H13" s="14" t="s">
         <v>32</v>
       </c>
       <c r="I13" s="11">
-        <v>13.99</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="J13" s="11">
         <f t="shared" si="0"/>
-        <v>41.97</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="8">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8">
+        <v>1</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="10">
+        <v>545512</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="11">
+        <v>9.99</v>
+      </c>
+      <c r="J14" s="11">
+        <f t="shared" si="0"/>
+        <v>9.99</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A15" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="8">
+        <v>2</v>
+      </c>
+      <c r="C15" s="8">
+        <v>2</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="10">
+        <v>585006</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="11">
+        <v>16.989999999999998</v>
+      </c>
+      <c r="J15" s="11">
+        <f t="shared" si="0"/>
+        <v>33.979999999999997</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A16" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="8">
+        <v>3</v>
+      </c>
+      <c r="C16" s="8">
+        <v>3</v>
+      </c>
+      <c r="D16" s="9">
+        <v>1</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="10">
+        <v>585004</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="11">
+        <v>13.99</v>
+      </c>
+      <c r="J16" s="11">
+        <f t="shared" si="0"/>
+        <v>41.97</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A17" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="13">
-        <v>12</v>
-      </c>
-      <c r="C14" s="13">
-        <v>12</v>
-      </c>
-      <c r="D14" s="9">
-        <v>1</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="13" t="s">
+      <c r="B17" s="13">
+        <v>12</v>
+      </c>
+      <c r="C17" s="13">
+        <v>12</v>
+      </c>
+      <c r="D17" s="9">
+        <v>1</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G17" s="17" t="s">
         <v>57</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="11">
-        <v>0.23</v>
-      </c>
-      <c r="J14" s="11">
-        <f t="shared" si="0"/>
-        <v>2.7600000000000002</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="8">
-        <v>4</v>
-      </c>
-      <c r="C15" s="8">
-        <v>4</v>
-      </c>
-      <c r="D15" s="9">
-        <v>1</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="11">
-        <v>0.3</v>
-      </c>
-      <c r="J15" s="11">
-        <f t="shared" si="0"/>
-        <v>1.2</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="L15" s="7"/>
-    </row>
-    <row r="16" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="8">
-        <v>100</v>
-      </c>
-      <c r="C16" s="8">
-        <v>12</v>
-      </c>
-      <c r="D16" s="9">
-        <v>100</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="11">
-        <v>1.17</v>
-      </c>
-      <c r="J16" s="11">
-        <f t="shared" si="0"/>
-        <v>1.17</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="L16" s="7"/>
-    </row>
-    <row r="17" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="8">
-        <v>5</v>
-      </c>
-      <c r="C17" s="8">
-        <v>3</v>
-      </c>
-      <c r="D17" s="9">
-        <v>5</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>69</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>15</v>
       </c>
       <c r="I17" s="11">
-        <v>2.4700000000000002</v>
+        <v>0.23</v>
       </c>
       <c r="J17" s="11">
         <f t="shared" si="0"/>
-        <v>2.4700000000000002</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="L17" s="7"/>
+        <v>2.7600000000000002</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="18" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="13">
-        <v>12</v>
-      </c>
-      <c r="C18" s="13">
-        <v>8</v>
+      <c r="A18" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="8">
+        <v>4</v>
+      </c>
+      <c r="C18" s="8">
+        <v>4</v>
       </c>
       <c r="D18" s="9">
         <v>1</v>
       </c>
-      <c r="E18" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>73</v>
+      <c r="E18" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>61</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>15</v>
       </c>
       <c r="I18" s="11">
-        <v>0.23</v>
+        <v>0.3</v>
       </c>
       <c r="J18" s="11">
         <f t="shared" si="0"/>
-        <v>2.7600000000000002</v>
-      </c>
-      <c r="K18" s="34" t="s">
-        <v>74</v>
+        <v>1.2</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="L18" s="7"/>
     </row>
     <row r="19" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" s="13">
-        <v>16</v>
-      </c>
-      <c r="C19" s="13">
+      <c r="A19" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="8">
+        <v>100</v>
+      </c>
+      <c r="C19" s="8">
         <v>12</v>
       </c>
       <c r="D19" s="9">
-        <v>1</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>76</v>
+        <v>100</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>15</v>
       </c>
       <c r="I19" s="11">
-        <v>0.27</v>
+        <v>1.17</v>
       </c>
       <c r="J19" s="11">
         <f t="shared" si="0"/>
-        <v>4.32</v>
-      </c>
-      <c r="K19" s="34" t="s">
-        <v>78</v>
+        <v>1.17</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="L19" s="7"/>
-      <c r="X19" s="7"/>
-      <c r="Y19" s="7"/>
-      <c r="Z19" s="7"/>
     </row>
     <row r="20" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="10" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B20" s="8">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C20" s="8">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D20" s="9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>81</v>
+        <v>68</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>15</v>
       </c>
       <c r="I20" s="11">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="J20" s="11">
+        <f t="shared" si="0"/>
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="L20" s="7"/>
+    </row>
+    <row r="21" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="13">
+        <v>12</v>
+      </c>
+      <c r="C21" s="13">
+        <v>8</v>
+      </c>
+      <c r="D21" s="9">
+        <v>1</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="11">
+        <v>0.23</v>
+      </c>
+      <c r="J21" s="11">
+        <f t="shared" si="0"/>
+        <v>2.7600000000000002</v>
+      </c>
+      <c r="K21" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="L21" s="7"/>
+    </row>
+    <row r="22" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="13">
+        <v>16</v>
+      </c>
+      <c r="C22" s="13">
+        <v>12</v>
+      </c>
+      <c r="D22" s="9">
+        <v>1</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="11">
+        <v>0.27</v>
+      </c>
+      <c r="J22" s="11">
+        <f t="shared" si="0"/>
+        <v>4.32</v>
+      </c>
+      <c r="K22" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="L22" s="7"/>
+      <c r="X22" s="7"/>
+      <c r="Y22" s="7"/>
+      <c r="Z22" s="7"/>
+    </row>
+    <row r="23" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="8">
+        <v>12</v>
+      </c>
+      <c r="C23" s="8">
+        <v>8</v>
+      </c>
+      <c r="D23" s="9">
+        <v>1</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="11">
         <v>0.37</v>
       </c>
-      <c r="J20" s="11">
+      <c r="J23" s="11">
         <f t="shared" si="0"/>
         <v>4.4399999999999995</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="K23" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="L20" s="7"/>
-      <c r="X20" s="7"/>
-      <c r="Y20" s="7"/>
-      <c r="Z20" s="7"/>
-    </row>
-    <row r="21" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="19" t="s">
+      <c r="L23" s="7"/>
+      <c r="X23" s="7"/>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7"/>
+    </row>
+    <row r="24" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="20">
+      <c r="B24" s="20">
         <v>6</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C24" s="20">
         <v>4</v>
       </c>
-      <c r="D21" s="21">
-        <v>1</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="20" t="s">
+      <c r="D24" s="21">
+        <v>1</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="G21" s="22" t="s">
+      <c r="G24" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="H21" s="23" t="s">
+      <c r="H24" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="I21" s="24">
+      <c r="I24" s="24">
         <v>0.48</v>
       </c>
-      <c r="J21" s="24">
+      <c r="J24" s="24">
         <f t="shared" si="0"/>
         <v>2.88</v>
       </c>
-      <c r="K21" s="25" t="s">
+      <c r="K24" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="L21" s="7"/>
-      <c r="X21" s="7"/>
-      <c r="Y21" s="7"/>
-      <c r="Z21" s="7"/>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A22" s="26" t="s">
+      <c r="L24" s="7"/>
+      <c r="X24" s="7"/>
+      <c r="Y24" s="7"/>
+      <c r="Z24" s="7"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A25" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="27">
+      <c r="B25" s="27">
         <v>100</v>
       </c>
-      <c r="C22" s="27">
+      <c r="C25" s="27">
         <v>4</v>
       </c>
-      <c r="D22" s="27">
+      <c r="D25" s="27">
         <v>100</v>
       </c>
-      <c r="E22" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="27" t="s">
+      <c r="E25" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="G22" s="28" t="s">
+      <c r="G25" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="H22" s="29" t="s">
+      <c r="H25" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="I22" s="30">
+      <c r="I25" s="30">
         <v>6.33</v>
       </c>
-      <c r="J22" s="30">
+      <c r="J25" s="30">
         <f t="shared" si="0"/>
         <v>6.33</v>
       </c>
-      <c r="K22" s="31" t="s">
+      <c r="K25" s="31" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A23" s="32" t="s">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A26" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="B23" s="27">
+      <c r="B26" s="27">
         <v>4</v>
       </c>
-      <c r="C23" s="27">
+      <c r="C26" s="27">
         <v>2</v>
       </c>
-      <c r="D23" s="27">
-        <v>1</v>
-      </c>
-      <c r="E23" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="27" t="s">
+      <c r="D26" s="27">
+        <v>1</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="G23" s="28" t="s">
+      <c r="G26" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="H23" s="33" t="s">
+      <c r="H26" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="I23" s="30">
+      <c r="I26" s="30">
         <v>0.96</v>
       </c>
-      <c r="J23" s="30">
+      <c r="J26" s="30">
         <f t="shared" si="0"/>
         <v>3.84</v>
       </c>
-      <c r="K23" s="31" t="s">
+      <c r="K26" s="31" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A24" s="38" t="s">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A27" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="B24" s="27">
-        <v>1</v>
-      </c>
-      <c r="C24" s="27">
-        <v>1</v>
-      </c>
-      <c r="D24" s="27">
-        <v>1</v>
-      </c>
-      <c r="E24" s="27" t="s">
+      <c r="B27" s="27">
+        <v>1</v>
+      </c>
+      <c r="C27" s="27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="F24" s="27" t="s">
+      <c r="F27" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="G24" s="36"/>
-      <c r="H24" s="33" t="s">
+      <c r="G27" s="36"/>
+      <c r="H27" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="I24" s="30">
+      <c r="I27" s="30">
         <v>11.75</v>
       </c>
-      <c r="J24" s="30">
+      <c r="J27" s="30">
         <f t="shared" si="0"/>
         <v>11.75</v>
       </c>
-      <c r="K24" s="31" t="s">
+      <c r="K27" s="31" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A25" s="38" t="s">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A28" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="B25" s="27">
-        <v>1</v>
-      </c>
-      <c r="C25" s="27">
-        <v>1</v>
-      </c>
-      <c r="D25" s="27">
-        <v>1</v>
-      </c>
-      <c r="E25" s="27" t="s">
+      <c r="B28" s="27">
+        <v>1</v>
+      </c>
+      <c r="C28" s="27">
+        <v>1</v>
+      </c>
+      <c r="D28" s="27">
+        <v>1</v>
+      </c>
+      <c r="E28" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="F25" s="27" t="s">
+      <c r="F28" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="G25" s="36"/>
-      <c r="H25" s="33" t="s">
+      <c r="G28" s="36"/>
+      <c r="H28" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="I25" s="30">
+      <c r="I28" s="30">
         <v>15.25</v>
       </c>
-      <c r="J25" s="30">
+      <c r="J28" s="30">
         <f t="shared" si="0"/>
         <v>15.25</v>
       </c>
-      <c r="K25" s="31" t="s">
+      <c r="K28" s="31" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A27" s="37" t="s">
+    <row r="30" spans="1:26" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A30" s="37" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="J28" s="35">
-        <f>SUM(J2:J25)</f>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="J31" s="35">
+        <f>SUM(J5:J28)</f>
         <v>240.37999999999994</v>
       </c>
-      <c r="K28" s="4" t="s">
+      <c r="K31" s="4" t="s">
         <v>94</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K13">
+  <autoFilter ref="A4:K16">
     <filterColumn colId="7">
       <filters>
         <filter val="Structural"/>
@@ -1858,22 +1957,26 @@
       <sortCondition ref="F1:F17"/>
     </sortState>
   </autoFilter>
+  <mergeCells count="2">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:F2"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K12" r:id="rId1"/>
-    <hyperlink ref="K13" r:id="rId2"/>
-    <hyperlink ref="K11" r:id="rId3"/>
-    <hyperlink ref="K3" r:id="rId4" location="90631A007"/>
-    <hyperlink ref="K5" r:id="rId5" location="96006A252"/>
-    <hyperlink ref="K6" r:id="rId6"/>
-    <hyperlink ref="K10" r:id="rId7" location="368=229"/>
-    <hyperlink ref="K7" r:id="rId8"/>
-    <hyperlink ref="K21" r:id="rId9" location="95947A007"/>
-    <hyperlink ref="K22" r:id="rId10" location="91251A076"/>
-    <hyperlink ref="K23" r:id="rId11" location="93330A252"/>
-    <hyperlink ref="K18" r:id="rId12" location="91780A162"/>
-    <hyperlink ref="K19" r:id="rId13" location="91780A164"/>
-    <hyperlink ref="K24" r:id="rId14"/>
-    <hyperlink ref="K25" r:id="rId15"/>
+    <hyperlink ref="K15" r:id="rId1"/>
+    <hyperlink ref="K16" r:id="rId2"/>
+    <hyperlink ref="K14" r:id="rId3"/>
+    <hyperlink ref="K6" r:id="rId4" location="90631A007"/>
+    <hyperlink ref="K8" r:id="rId5" location="96006A252"/>
+    <hyperlink ref="K9" r:id="rId6"/>
+    <hyperlink ref="K13" r:id="rId7" location="368=229"/>
+    <hyperlink ref="K10" r:id="rId8"/>
+    <hyperlink ref="K24" r:id="rId9" location="95947A007"/>
+    <hyperlink ref="K25" r:id="rId10" location="91251A076"/>
+    <hyperlink ref="K26" r:id="rId11" location="93330A252"/>
+    <hyperlink ref="K21" r:id="rId12" location="91780A162"/>
+    <hyperlink ref="K22" r:id="rId13" location="91780A164"/>
+    <hyperlink ref="K27" r:id="rId14"/>
+    <hyperlink ref="K28" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId16"/>

</xml_diff>